<commit_message>
"Laboratorio 4 - Entrega final"
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4.xlsx
+++ b/Docs/Tablas Lab 4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 04 - Ordenamientos Iterativos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omelo_ifi09dn\OneDrive\Documentos\U\segundo semestre\EDA\ISIS1225-LabSorts-S07-G06\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E197636-5D23-49AC-AB0F-C814FF421F77}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C6ACB9-C519-4433-87FA-DB8B808E4446}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="5" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,12 +110,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -142,6 +148,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -459,7 +468,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -664,22 +673,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>687.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>5578.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>23796.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>84609.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>445359.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>398218.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>70</c:v>
@@ -832,34 +841,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>812.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5171.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>26546.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>126609.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>398218.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>524828.125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>923046.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>1447875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55</c:v>
+                  <c:v>2370921.875</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>3818796.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -999,34 +1008,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>46.875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>187.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>421.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>796.875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>806.875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>816.875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>826.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>836.875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
+                  <c:v>846.875</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>856.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1374,7 +1383,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1579,7 +1588,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>116312.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>60</c:v>
@@ -1708,34 +1717,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>119781.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>119785.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>119789.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>239574.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>359363.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42</c:v>
+                  <c:v>598938.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68</c:v>
+                  <c:v>958302</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110</c:v>
+                  <c:v>1557240.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>2515542.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1747,34 +1756,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>119781.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>119785.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>119789.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>239574.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>359363.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42</c:v>
+                  <c:v>598938.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68</c:v>
+                  <c:v>958302</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110</c:v>
+                  <c:v>1557240.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>2515542.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1914,34 +1923,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>5437.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>5480.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>5490.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>5500.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
+                  <c:v>5510.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>118</c:v>
+                  <c:v>5520.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>128</c:v>
+                  <c:v>5530.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>138</c:v>
+                  <c:v>5540.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>148</c:v>
+                  <c:v>5550.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>5560.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2289,7 +2298,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2495,22 +2504,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>687.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>5578.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>23796.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>84609.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>445359.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>398218.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>70</c:v>
@@ -2663,7 +2672,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>116312.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>60</c:v>
@@ -3033,7 +3042,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3234,34 +3243,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>812.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5171.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>26546.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>126609.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>398218.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>524828.125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>923046.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>1447875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55</c:v>
+                  <c:v>2370921.875</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>3818796.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3402,34 +3411,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>119781.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>119785.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>119789.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>239574.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>359363.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42</c:v>
+                  <c:v>598938.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68</c:v>
+                  <c:v>958302</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110</c:v>
+                  <c:v>1557240.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>2515542.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3772,7 +3781,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3973,34 +3982,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>46.875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>187.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>421.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>796.875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>806.875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>816.875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>826.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>836.875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
+                  <c:v>846.875</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>856.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4141,34 +4150,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>5437.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>5480.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>5490.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>5500.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
+                  <c:v>5510.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>118</c:v>
+                  <c:v>5520.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>128</c:v>
+                  <c:v>5530.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>138</c:v>
+                  <c:v>5540.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>148</c:v>
+                  <c:v>5550.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>5560.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7286,7 +7295,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="67" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7297,7 +7306,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="67" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7308,7 +7317,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="67" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7319,7 +7328,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{662C0436-FCD4-45AD-AA7D-093158D92847}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="67" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7330,7 +7339,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="67" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7341,7 +7350,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9307015" cy="6075149"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7374,7 +7383,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9307015" cy="6075149"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7407,7 +7416,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9307015" cy="6075149"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7440,7 +7449,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9307015" cy="6075149"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7473,7 +7482,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9307015" cy="6075149"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7529,7 +7538,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7827,19 +7836,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="34.1171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.52734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.76171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -7853,100 +7862,94 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
       <c r="B2" s="4">
-        <v>10</v>
+        <v>687.5</v>
       </c>
       <c r="C2" s="4">
-        <v>1</v>
+        <v>812.5</v>
       </c>
       <c r="D2" s="4">
-        <v>4</v>
+        <v>46.875</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
       <c r="B3" s="4">
-        <v>20</v>
+        <v>5578.125</v>
       </c>
       <c r="C3" s="4">
-        <v>2</v>
+        <v>5171.875</v>
       </c>
       <c r="D3" s="4">
-        <f>D2+15</f>
-        <v>19</v>
+        <v>187.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
       <c r="B4" s="4">
-        <v>30</v>
+        <v>23796.875</v>
       </c>
       <c r="C4" s="4">
-        <f>C3+C2</f>
-        <v>3</v>
+        <v>26546.875</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">D3+10</f>
-        <v>29</v>
+        <v>421.875</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
       <c r="B5" s="4">
-        <v>40</v>
+        <v>84609.375</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>5</v>
+        <v>126609.375</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <v>796.875</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
       <c r="B6" s="4">
-        <v>50</v>
+        <v>445359.375</v>
       </c>
       <c r="C6" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <v>398218.75</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" ref="D4:D11" si="0">D5+10</f>
+        <v>806.875</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
       <c r="B7" s="4">
-        <v>60</v>
+        <v>398218.75</v>
       </c>
       <c r="C7" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f t="shared" ref="C5:C11" si="1">C6+C5</f>
+        <v>524828.125</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>816.875</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
@@ -7955,14 +7958,14 @@
       </c>
       <c r="C8" s="4">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>923046.875</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>826.875</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
@@ -7971,14 +7974,14 @@
       </c>
       <c r="C9" s="4">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>1447875</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>79</v>
+        <v>836.875</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
@@ -7987,14 +7990,14 @@
       </c>
       <c r="C10" s="4">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>2370921.875</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>846.875</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>512000</v>
       </c>
@@ -8003,14 +8006,14 @@
       </c>
       <c r="C11" s="4">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>3818796.875</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>856.875</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -8024,21 +8027,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
       <c r="B15" s="4">
-        <v>50</v>
+        <v>116312.5</v>
       </c>
       <c r="C15" s="4">
-        <v>2</v>
+        <v>119781.25</v>
       </c>
       <c r="D15" s="4">
-        <v>35</v>
+        <v>5437.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
@@ -8050,10 +8053,10 @@
       </c>
       <c r="D16" s="4">
         <f>D15+43</f>
-        <v>78</v>
+        <v>5480.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
@@ -8062,14 +8065,14 @@
       </c>
       <c r="C17" s="4">
         <f t="shared" ref="C17:C24" si="2">C16+C15</f>
-        <v>6</v>
+        <v>119785.25</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" ref="D17:D24" si="3">D16+10</f>
-        <v>88</v>
+        <v>5490.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
@@ -8078,14 +8081,14 @@
       </c>
       <c r="C18" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>119789.25</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="3"/>
-        <v>98</v>
+        <v>5500.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
@@ -8094,14 +8097,14 @@
       </c>
       <c r="C19" s="4">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>239574.5</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="3"/>
-        <v>108</v>
+        <v>5510.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
@@ -8110,14 +8113,14 @@
       </c>
       <c r="C20" s="4">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>359363.75</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="3"/>
-        <v>118</v>
+        <v>5520.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
@@ -8126,14 +8129,14 @@
       </c>
       <c r="C21" s="4">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>598938.25</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="3"/>
-        <v>128</v>
+        <v>5530.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
@@ -8142,14 +8145,14 @@
       </c>
       <c r="C22" s="4">
         <f t="shared" si="2"/>
-        <v>68</v>
+        <v>958302</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="3"/>
-        <v>138</v>
+        <v>5540.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
@@ -8158,14 +8161,14 @@
       </c>
       <c r="C23" s="4">
         <f t="shared" si="2"/>
-        <v>110</v>
+        <v>1557240.25</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="3"/>
-        <v>148</v>
+        <v>5550.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>512000</v>
       </c>
@@ -8174,11 +8177,11 @@
       </c>
       <c r="C24" s="4">
         <f t="shared" si="2"/>
-        <v>178</v>
+        <v>2515542.25</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="3"/>
-        <v>158</v>
+        <v>5560.5</v>
       </c>
     </row>
   </sheetData>
@@ -8191,12 +8194,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8411,15 +8411,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8444,10 +8448,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>